<commit_message>
Add ability to start/stop and configurable preheat when starting a cycle. - Required adding a new `EncoderShim` to intercept all encoder interactions so that we can know a long-press has occurred. - Preheat is indicated by a title bar widget. - Preheat start/stop with long-press is a toggle of current state, it is not impacted in any way by what operation was being done (ie, you start a preheat while stopping a spin cycle with a long-press) - Made encoder inversion work in new shim - Switch StealthChop transition point into a simple on/off for StealthChop as a whole.   There isn't any point in having stealthchop enabled at all if we cannot use it across full motor speed range, as the transition is abbrupt, and causes a large jerk.
</commit_message>
<xml_diff>
--- a/TMC_calculations.xlsx
+++ b/TMC_calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a4184be35593cb15/Documents/PlatformIO/Projects/KiwiBoardFirmware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{83FAD72C-7206-4077-9009-AB390C7DA6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C13CC59-CA9C-4A3C-9D9F-641B5FFC2621}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{83FAD72C-7206-4077-9009-AB390C7DA6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5BAEC19-F038-4B4A-B70A-E577FBFACF85}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D1DB0E69-0973-44C2-9B0D-55F2DAAC8229}"/>
   </bookViews>
@@ -212,6 +212,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -527,7 +531,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>